<commit_message>
Atualizado gitignore e scrum
</commit_message>
<xml_diff>
--- a/scrum/financeiraJavaFX.xlsx
+++ b/scrum/financeiraJavaFX.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">SCRUM – financeiraJavaFX</t>
   </si>
@@ -64,37 +64,46 @@
     <t xml:space="preserve">Resolver DAO</t>
   </si>
   <si>
+    <t xml:space="preserve">validaçoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atualiza DAO quando edita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parcelas Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validações data e dinheiro (Como Classe de Eventos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nova Operação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validações data e dinheiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novo Empréstimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validações cria usuário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Persistencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerador Parcelas</t>
+  </si>
+  <si>
     <t xml:space="preserve">GUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atualiza DAO quando edita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parcelas Valor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nova Operação</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Novo Empréstimo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">validações cria usuário</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Persistencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerador Parcelas</t>
   </si>
 </sst>
 </file>
@@ -144,7 +153,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +200,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF33FF99"/>
         <bgColor rgb="FF66FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -228,7 +243,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,6 +285,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,10 +369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -362,7 +381,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.0102040816327"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.8367346938776"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="36.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.780612244898"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8673469387755"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
@@ -431,39 +450,51 @@
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="F6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>24</v>
-      </c>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
[Sync] Consertando validacao de textfield com data e valores
</commit_message>
<xml_diff>
--- a/scrum/financeiraJavaFX.xlsx
+++ b/scrum/financeiraJavaFX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="financeiraJavaFX" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">SCRUM – financeiraJavaFX</t>
   </si>
@@ -76,19 +76,22 @@
     <t xml:space="preserve">validações data e dinheiro (Como Classe de Eventos)</t>
   </si>
   <si>
+    <t xml:space="preserve">validações data</t>
+  </si>
+  <si>
     <t xml:space="preserve">UML</t>
   </si>
   <si>
     <t xml:space="preserve">Nova Operação</t>
   </si>
   <si>
-    <t xml:space="preserve">validações data e dinheiro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Model</t>
   </si>
   <si>
     <t xml:space="preserve">Novo Empréstimo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validacao dinheiro</t>
   </si>
   <si>
     <t xml:space="preserve">Controller</t>
@@ -118,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,18 +143,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -371,34 +378,52 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.4795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.1479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -453,18 +478,19 @@
       <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="0"/>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
@@ -473,26 +499,29 @@
       <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0"/>
     </row>

</xml_diff>